<commit_message>
Updated code with Create Order for Customer and Store
</commit_message>
<xml_diff>
--- a/TestData/LoginTestData/login.xlsx
+++ b/TestData/LoginTestData/login.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\POM_for_Bottle\WebApp\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\POM_for_Bottle\WebApp\TestData\LoginTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C69090DA-8598-4FC5-9A77-800209B60AD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2F37050-DAF7-4F12-B5D5-B0C1312B81CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="15">
   <si>
     <t>username</t>
   </si>
@@ -53,9 +53,6 @@
     <t>Test@1823</t>
   </si>
   <si>
-    <t>2 validation errors detected: Value at 'userAlias' failed to satisfy constraint: Member must satisfy regular expression pattern: [\p{L}\p{M}\p{S}\p{N}\p{P}]+; Value at 'userName' failed to satisfy constraint: Member must satisfy regular expression pattern: [\p{L}\p{M}\p{S}\p{N}\p{P}]+</t>
-  </si>
-  <si>
     <t>frugal @latido.com.np</t>
   </si>
   <si>
@@ -71,7 +68,7 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>2 v  alidation errors detected: Value at 'userAlias' failed to satisfy constraint: Member must satisfy regular expression pattern: [\p{L}\p{M}\p{S}\p{N}\p{P}]+; Value at 'userName' failed to satisfy constraint: Member must satisfy regular expression pattern: [\p{L}\p{M}\p{S}\p{N}\p{P}]+</t>
+    <t>Please check username</t>
   </si>
 </sst>
 </file>
@@ -1026,7 +1023,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1047,24 +1044,24 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1101,7 +1098,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1110,7 +1107,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1144,10 +1141,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1155,10 +1152,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated code till Inventory Dashboard
</commit_message>
<xml_diff>
--- a/TestData/LoginTestData/login.xlsx
+++ b/TestData/LoginTestData/login.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\POM_for_Bottle\WebApp\TestData\LoginTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2F37050-DAF7-4F12-B5D5-B0C1312B81CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F25F9FC4-E80F-4946-A999-82C8836B4DC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="23">
   <si>
     <t>username</t>
   </si>
@@ -44,9 +44,6 @@
     <t>OVERVIEW</t>
   </si>
   <si>
-    <t>Incorrect username or password.</t>
-  </si>
-  <si>
     <t>Test@103</t>
   </si>
   <si>
@@ -69,13 +66,40 @@
   </si>
   <si>
     <t>Please check username</t>
+  </si>
+  <si>
+    <t>rohit13@latido.com.np</t>
+  </si>
+  <si>
+    <t>Frugal@123</t>
+  </si>
+  <si>
+    <t>Test@124</t>
+  </si>
+  <si>
+    <t>Test@1824</t>
+  </si>
+  <si>
+    <t>Test@1825</t>
+  </si>
+  <si>
+    <t>frugal@latido.com</t>
+  </si>
+  <si>
+    <t>f rugallatido.com.np</t>
+  </si>
+  <si>
+    <t>Test@3543</t>
+  </si>
+  <si>
+    <t>Test@5263</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -219,6 +243,14 @@
     <font>
       <sz val="10"/>
       <name val="Roboto"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="33">
@@ -518,7 +550,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -561,13 +593,15 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -601,6 +635,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -922,10 +957,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22:E23"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -963,19 +998,45 @@
         <v>5</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{0B9CA44F-85B4-4D86-AB90-98DDC57CC5F5}"/>
+    <hyperlink ref="B5" r:id="rId2" xr:uid="{46C9A5DA-7546-40F3-A325-3FBAC3D4E52C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B02F724E-BA7E-41E4-8CFA-C18066E75053}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -996,10 +1057,10 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
         <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1007,23 +1068,50 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{1D1263DD-78FE-4FAC-8D19-6B4C8B222166}"/>
+    <hyperlink ref="B5" r:id="rId2" display="Test@123" xr:uid="{9A4629CA-E1C0-4896-A4A3-5720B486F23D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90193C80-F867-4439-BACC-918286CAAFE4}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1044,39 +1132,64 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="A4" r:id="rId1" xr:uid="{E3C302A5-69CA-4827-BADF-0CF6BAAF5E75}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11FE210F-88D5-4BDA-800B-A9813C424A2E}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1095,32 +1208,49 @@
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B21B9964-019A-427F-81C6-BB140FFD3035}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1141,10 +1271,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1152,10 +1282,26 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>